<commit_message>
Stationarity test with two similar subtasks: changes made inside stationarity_test/stationarity test with subtask_1
</commit_message>
<xml_diff>
--- a/Brightkite_neew/p12-brightkite-0ms-annot.xlsx
+++ b/Brightkite_neew/p12-brightkite-0ms-annot.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\Brightkite_neew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52118499-3FB7-4F57-89ED-610F4F332C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1830C53C-D304-40C8-8443-EEFDB84DB5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet_1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="121">
   <si>
     <t>proposition</t>
   </si>
@@ -382,6 +383,12 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user finds some trends looking at different areas from a high zoom level and comes up with some hypotheses </t>
+  </si>
+  <si>
+    <t>Users zooms into particular locations to see if the trends he/she found contradicts or not.</t>
   </si>
 </sst>
 </file>
@@ -745,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection sqref="A1:J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3138,6 +3145,2411 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B243327-EB67-4BD7-ADC7-1B03DFC28CDA}">
+  <dimension ref="A1:J90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104" customWidth="1"/>
+    <col min="2" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="56.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.7118055555555602E-2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.7222222222222201E-2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.73148148148148E-2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.7557870370370401E-2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.7743055555555599E-2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.7777777777777799E-2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.8009259259259301E-2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.8148148148148201E-2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.83449074074074E-2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.8460648148148202E-2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.8495370370370402E-2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.8587962962963001E-2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.8726851851851901E-2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.8784722222222199E-2</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.90277777777778E-2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.9108796296296301E-2</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.9189814814814798E-2</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.9259259259259299E-2</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.9282407407407401E-2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1.9537037037036999E-2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.02083333333333E-2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.0312500000000001E-2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2.1006944444444401E-2</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2.12037037037037E-2</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2.1250000000000002E-2</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2.13425925925926E-2</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2.1400462962963E-2</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>2.20601851851852E-2</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.2314814814814801E-2</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2.2337962962963E-2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2.2662037037037001E-2</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2.2685185185185201E-2</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2.3009259259259299E-2</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2.3136574074074101E-2</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2.3217592592592599E-2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.3287037037036998E-2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2">
+        <v>2.3530092592592599E-2</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>2.3587962962963002E-2</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2.36458333333333E-2</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2.4594907407407399E-2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2.4872685185185199E-2</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2.5590277777777799E-2</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>2.58101851851852E-2</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2</v>
+      </c>
+      <c r="H45" s="2">
+        <v>2.58796296296296E-2</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+      <c r="H46" s="2">
+        <v>2.6145833333333299E-2</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47" s="2">
+        <v>2.61921296296296E-2</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>2.62268518518519E-2</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>2.6319444444444399E-2</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+      <c r="H50" s="2">
+        <v>2.6354166666666699E-2</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2.6412037037037001E-2</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="2">
+        <v>2.6608796296296301E-2</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
+        <v>2.6689814814814802E-2</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2</v>
+      </c>
+      <c r="H54" s="2">
+        <v>2.6759259259259299E-2</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2</v>
+      </c>
+      <c r="H55" s="2">
+        <v>2.6817129629629601E-2</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <v>2.68402777777778E-2</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2</v>
+      </c>
+      <c r="H57" s="2">
+        <v>2.7210648148148098E-2</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>2</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H58" s="2">
+        <v>2.7268518518518501E-2</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2">
+        <v>2.7418981481481499E-2</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2">
+        <v>2.7523148148148099E-2</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="2">
+        <v>2.7581018518518501E-2</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+      <c r="H62" s="2">
+        <v>2.77083333333333E-2</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H63" s="2">
+        <v>2.8113425925925899E-2</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>2</v>
+      </c>
+      <c r="H64" s="2">
+        <v>2.81828703703704E-2</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>2</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2.8240740740740702E-2</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>2</v>
+      </c>
+      <c r="H66" s="2">
+        <v>2.8287037037036999E-2</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H67" s="2">
+        <v>2.83564814814815E-2</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
+      <c r="H68" s="2">
+        <v>2.8888888888888901E-2</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>2</v>
+      </c>
+      <c r="H69" s="2">
+        <v>2.8969907407407399E-2</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2">
+        <v>2.95601851851852E-2</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>94</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2">
+        <v>3.0104166666666699E-2</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2">
+        <v>3.0289351851851901E-2</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
+      <c r="H73" s="2">
+        <v>3.0347222222222199E-2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
+      <c r="H74" s="2">
+        <v>3.0347222222222199E-2</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="H75" s="2">
+        <v>3.03935185185185E-2</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1">
+        <v>2</v>
+      </c>
+      <c r="H76" s="2">
+        <v>3.0636574074074101E-2</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>2</v>
+      </c>
+      <c r="H77" s="2">
+        <v>3.0914351851851901E-2</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78" s="2">
+        <v>3.10763888888889E-2</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1">
+        <v>2</v>
+      </c>
+      <c r="H79" s="2">
+        <v>3.11458333333333E-2</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1">
+        <v>2</v>
+      </c>
+      <c r="H80" s="2">
+        <v>3.14930555555556E-2</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>2</v>
+      </c>
+      <c r="H81" s="2">
+        <v>3.1574074074074102E-2</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1">
+        <v>2</v>
+      </c>
+      <c r="H82" s="2">
+        <v>3.1793981481481499E-2</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2">
+        <v>3.1851851851851902E-2</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2">
+        <v>3.1875000000000001E-2</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2">
+        <v>3.2592592592592597E-2</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1">
+        <v>1</v>
+      </c>
+      <c r="H86" s="2">
+        <v>3.4178240740740697E-2</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2">
+        <v>3.4328703703703702E-2</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1">
+        <v>1</v>
+      </c>
+      <c r="H88" s="2">
+        <v>3.5081018518518498E-2</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1">
+        <v>1</v>
+      </c>
+      <c r="H89" s="2">
+        <v>3.5914351851851899E-2</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+      <c r="F90" s="1">
+        <v>1</v>
+      </c>
+      <c r="H90" s="2">
+        <v>3.5983796296296298E-2</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stationarity test modified: all subtasks added for pymann kendall
</commit_message>
<xml_diff>
--- a/Brightkite_neew/p12-brightkite-0ms-annot.xlsx
+++ b/Brightkite_neew/p12-brightkite-0ms-annot.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\Brightkite_neew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1830C53C-D304-40C8-8443-EEFDB84DB5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F52916C-6993-47C5-A2D0-CB42C5738391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet_1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1(2)" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet_1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="121">
   <si>
     <t>proposition</t>
   </si>
@@ -749,6 +750,2413 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFFF227-5704-44D0-93BE-57D8B515F4A2}">
+  <dimension ref="A1:J90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J85" sqref="J85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104" customWidth="1"/>
+    <col min="2" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="56.42578125" customWidth="1"/>
+    <col min="11" max="1025" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.7118055555555602E-2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.7222222222222201E-2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.73148148148148E-2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.7557870370370401E-2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.7743055555555599E-2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.7777777777777799E-2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.8009259259259301E-2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.8148148148148201E-2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.83449074074074E-2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.8460648148148202E-2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.8495370370370402E-2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.8587962962963001E-2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.8726851851851901E-2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.8784722222222199E-2</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.90277777777778E-2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.9108796296296301E-2</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.9189814814814798E-2</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.9259259259259299E-2</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.9282407407407401E-2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1.9537037037036999E-2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.02083333333333E-2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.0312500000000001E-2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2.1006944444444401E-2</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2.12037037037037E-2</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2.1250000000000002E-2</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2.13425925925926E-2</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2.1400462962963E-2</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>2.20601851851852E-2</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.2314814814814801E-2</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2.2337962962963E-2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2.2662037037037001E-2</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2.2685185185185201E-2</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2.3009259259259299E-2</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2.3136574074074101E-2</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2.3217592592592599E-2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.3287037037036998E-2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2">
+        <v>2.3530092592592599E-2</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>2.3587962962963002E-2</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2.36458333333333E-2</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2.4594907407407399E-2</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2.4872685185185199E-2</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2.5590277777777799E-2</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="J43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>2.58101851851852E-2</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2</v>
+      </c>
+      <c r="H45" s="2">
+        <v>2.58796296296296E-2</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+      <c r="H46" s="2">
+        <v>2.6145833333333299E-2</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47" s="2">
+        <v>2.61921296296296E-2</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>2.62268518518519E-2</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>2.6319444444444399E-2</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+      <c r="H50" s="2">
+        <v>2.6354166666666699E-2</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2.6412037037037001E-2</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="2">
+        <v>2.6608796296296301E-2</v>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
+        <v>2.6689814814814802E-2</v>
+      </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2</v>
+      </c>
+      <c r="H54" s="2">
+        <v>2.6759259259259299E-2</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2</v>
+      </c>
+      <c r="H55" s="2">
+        <v>2.6817129629629601E-2</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <v>2.68402777777778E-2</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2</v>
+      </c>
+      <c r="H57" s="2">
+        <v>2.7210648148148098E-2</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>2</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H58" s="2">
+        <v>2.7268518518518501E-2</v>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2">
+        <v>2.7418981481481499E-2</v>
+      </c>
+      <c r="I59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2">
+        <v>2.7523148148148099E-2</v>
+      </c>
+      <c r="I60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="2">
+        <v>2.7581018518518501E-2</v>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+      <c r="H62" s="2">
+        <v>2.77083333333333E-2</v>
+      </c>
+      <c r="I62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H63" s="2">
+        <v>2.8113425925925899E-2</v>
+      </c>
+      <c r="I63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>2</v>
+      </c>
+      <c r="H64" s="2">
+        <v>2.81828703703704E-2</v>
+      </c>
+      <c r="I64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>2</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2.8240740740740702E-2</v>
+      </c>
+      <c r="I65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>2</v>
+      </c>
+      <c r="H66" s="2">
+        <v>2.8287037037036999E-2</v>
+      </c>
+      <c r="I66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H67" s="2">
+        <v>2.83564814814815E-2</v>
+      </c>
+      <c r="I67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
+      <c r="H68" s="2">
+        <v>2.8888888888888901E-2</v>
+      </c>
+      <c r="I68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>2</v>
+      </c>
+      <c r="H69" s="2">
+        <v>2.8969907407407399E-2</v>
+      </c>
+      <c r="I69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2">
+        <v>2.95601851851852E-2</v>
+      </c>
+      <c r="I70">
+        <v>4</v>
+      </c>
+      <c r="J70" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>94</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2">
+        <v>3.0104166666666699E-2</v>
+      </c>
+      <c r="I71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2">
+        <v>3.0289351851851901E-2</v>
+      </c>
+      <c r="I72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
+      <c r="H73" s="2">
+        <v>3.0347222222222199E-2</v>
+      </c>
+      <c r="I73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
+      <c r="H74" s="2">
+        <v>3.0347222222222199E-2</v>
+      </c>
+      <c r="I74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="H75" s="2">
+        <v>3.03935185185185E-2</v>
+      </c>
+      <c r="I75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1">
+        <v>2</v>
+      </c>
+      <c r="H76" s="2">
+        <v>3.0636574074074101E-2</v>
+      </c>
+      <c r="I76">
+        <v>4</v>
+      </c>
+      <c r="J76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>2</v>
+      </c>
+      <c r="H77" s="2">
+        <v>3.0914351851851901E-2</v>
+      </c>
+      <c r="I77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78" s="2">
+        <v>3.10763888888889E-2</v>
+      </c>
+      <c r="I78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1">
+        <v>2</v>
+      </c>
+      <c r="H79" s="2">
+        <v>3.11458333333333E-2</v>
+      </c>
+      <c r="I79">
+        <v>5</v>
+      </c>
+      <c r="J79" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1">
+        <v>2</v>
+      </c>
+      <c r="H80" s="2">
+        <v>3.14930555555556E-2</v>
+      </c>
+      <c r="I80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>2</v>
+      </c>
+      <c r="H81" s="2">
+        <v>3.1574074074074102E-2</v>
+      </c>
+      <c r="I81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1">
+        <v>2</v>
+      </c>
+      <c r="H82" s="2">
+        <v>3.1793981481481499E-2</v>
+      </c>
+      <c r="I82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2">
+        <v>3.1851851851851902E-2</v>
+      </c>
+      <c r="I83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2">
+        <v>3.1875000000000001E-2</v>
+      </c>
+      <c r="I84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2">
+        <v>3.2592592592592597E-2</v>
+      </c>
+      <c r="I85">
+        <v>5</v>
+      </c>
+      <c r="J85" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1">
+        <v>1</v>
+      </c>
+      <c r="H86" s="2">
+        <v>3.4178240740740697E-2</v>
+      </c>
+      <c r="I86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2">
+        <v>3.4328703703703702E-2</v>
+      </c>
+      <c r="I87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1">
+        <v>1</v>
+      </c>
+      <c r="H88" s="2">
+        <v>3.5081018518518498E-2</v>
+      </c>
+      <c r="I88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1">
+        <v>1</v>
+      </c>
+      <c r="H89" s="2">
+        <v>3.5914351851851899E-2</v>
+      </c>
+      <c r="I89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+      <c r="F90" s="1">
+        <v>1</v>
+      </c>
+      <c r="H90" s="2">
+        <v>3.5983796296296298E-2</v>
+      </c>
+      <c r="I90">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
@@ -3149,12 +5557,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B243327-EB67-4BD7-ADC7-1B03DFC28CDA}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>